<commit_message>
update sdPublisher field to use Data Catalog type
</commit_message>
<xml_diff>
--- a/data/2024_05_14_RepoMetaCuration.xlsx
+++ b/data/2024_05_14_RepoMetaCuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtsueng\Anaconda3\envs\nde\nde_meta_batch_converter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080FED36-B54A-4A02-BB78-E3A19F64A235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E209C3-DA95-4CFE-A887-3F4F071025C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resource_base" sheetId="1" r:id="rId1"/>
@@ -1768,7 +1768,7 @@
   </sheetPr>
   <dimension ref="A1:W998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -6194,8 +6194,8 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6570,7 +6570,7 @@
         <v>197</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>198</v>
@@ -6617,7 +6617,7 @@
         <v>197</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>198</v>
@@ -6664,7 +6664,7 @@
         <v>197</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>198</v>

</xml_diff>